<commit_message>
Update ~ SnowMountain Field (Temp)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/SnowMountain.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/SnowMountain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A869820-49E0-426A-B44A-DBF148EC45E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989A28F-0822-469C-9A5E-15D9F8B5A1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" activeTab="3" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" firstSheet="8" activeTab="17" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -12737,7 +12737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="217">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -14498,6 +14498,30 @@
   </si>
   <si>
     <t>SnowMountainShadowGame</t>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Get Ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Remove Ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Get Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Remove Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결혼반지함이 사라진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Disappear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -15535,7 +15559,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="A2:H13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -15612,7 +15636,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>136</v>
@@ -15629,7 +15653,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -15640,7 +15664,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -15651,7 +15675,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -15680,7 +15704,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -15752,7 +15776,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>136</v>
@@ -15769,7 +15793,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -15780,7 +15804,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -15791,7 +15815,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -15817,10 +15841,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A805CFC-5BC1-4539-96EF-5EC0BB405817}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -15899,7 +15923,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>143</v>
@@ -15916,7 +15940,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>144</v>
@@ -15927,7 +15951,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>145</v>
@@ -15938,7 +15962,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>146</v>
@@ -15955,9 +15979,14 @@
         <v>148</v>
       </c>
       <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -15970,10 +15999,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9550A747-66C4-4F2A-9280-B10283B8F5BB}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -16045,7 +16074,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>146</v>
@@ -16071,11 +16100,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
+    <row r="7" spans="1:6">
+      <c r="C7">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16088,9 +16117,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFEE5DE-40D5-488A-A079-CB1D1BD4C3A8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
@@ -16161,7 +16192,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>149</v>
@@ -16176,11 +16207,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
+    <row r="6" spans="1:6">
+      <c r="C6">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16194,10 +16225,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C939AC5-8089-4FE1-8A0F-7CEDBDFFF404}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -16276,7 +16307,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>149</v>
@@ -16293,102 +16324,175 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>154</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>150</v>
       </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>151</v>
       </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>161</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>162</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>156</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>157</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
         <v>152</v>
       </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>153</v>
       </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>160</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -18037,7 +18141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C200D7-C0B4-4460-8B8F-6B50F370EC7E}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update ~ SnowMountain Field (Temp) (#86)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/SnowMountain.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/SnowMountain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A869820-49E0-426A-B44A-DBF148EC45E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989A28F-0822-469C-9A5E-15D9F8B5A1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" activeTab="3" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" firstSheet="8" activeTab="17" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="41" r:id="rId1"/>
@@ -12737,7 +12737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="217">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -14498,6 +14498,30 @@
   </si>
   <si>
     <t>SnowMountainShadowGame</t>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Get Ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Remove Ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Get Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Remove Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결혼반지함이 사라진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, 0.5, name=Stage 1/4 SnowMountain/Ring/Disappear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -15535,7 +15559,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="A2:H13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -15612,7 +15636,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>136</v>
@@ -15629,7 +15653,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -15640,7 +15664,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -15651,7 +15675,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -15680,7 +15704,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -15752,7 +15776,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>136</v>
@@ -15769,7 +15793,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -15780,7 +15804,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -15791,7 +15815,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -15817,10 +15841,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A805CFC-5BC1-4539-96EF-5EC0BB405817}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -15899,7 +15923,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>143</v>
@@ -15916,7 +15940,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>144</v>
@@ -15927,7 +15951,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>145</v>
@@ -15938,7 +15962,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>146</v>
@@ -15955,9 +15979,14 @@
         <v>148</v>
       </c>
       <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -15970,10 +15999,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9550A747-66C4-4F2A-9280-B10283B8F5BB}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -16045,7 +16074,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>146</v>
@@ -16071,11 +16100,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
+    <row r="7" spans="1:6">
+      <c r="C7">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16088,9 +16117,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFEE5DE-40D5-488A-A079-CB1D1BD4C3A8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
@@ -16161,7 +16192,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>149</v>
@@ -16176,11 +16207,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
+    <row r="6" spans="1:6">
+      <c r="C6">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16194,10 +16225,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C939AC5-8089-4FE1-8A0F-7CEDBDFFF404}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -16276,7 +16307,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>149</v>
@@ -16293,102 +16324,175 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>154</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>150</v>
       </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>151</v>
       </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>161</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>162</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>156</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>157</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
         <v>152</v>
       </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>153</v>
       </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>160</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -18037,7 +18141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C200D7-C0B4-4460-8B8F-6B50F370EC7E}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix Snowmountain Interaction (#111)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/SnowMountain.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/SnowMountain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EE790D-D628-466C-A57C-3917744B2FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DE7E2D-2DA8-489E-941F-0B876782947D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -4598,7 +4598,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="226">
   <si>
     <t>파일명</t>
   </si>
@@ -11911,8 +11911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="B10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -12054,12 +12054,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
-      <c r="C10" s="1">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
@@ -15316,7 +15312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -18819,7 +18815,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -20522,8 +20520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -21039,9 +21037,7 @@
       <c r="D38" s="1">
         <v>4</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="16.5" customHeight="1">
       <c r="A39" s="3"/>

</xml_diff>